<commit_message>
Adds task-preprocessed version of KNN
</commit_message>
<xml_diff>
--- a/ResearchPlanningReport/Data.xlsx
+++ b/ResearchPlanningReport/Data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Dev\Experiments\ResearchPlanningReport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92597776-FD49-4F7C-930E-A4012A63547E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFBECB0-EEB5-4EC2-B18F-2000714A96CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26895" yWindow="2850" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V0" sheetId="1" r:id="rId1"/>
     <sheet name="V0CE" sheetId="4" r:id="rId2"/>
-    <sheet name="Generic" sheetId="2" r:id="rId3"/>
-    <sheet name="EverythingOneDevice" sheetId="3" r:id="rId4"/>
+    <sheet name="V2CE" sheetId="5" r:id="rId3"/>
+    <sheet name="Generic" sheetId="2" r:id="rId4"/>
+    <sheet name="EverythingOneDevice" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="59">
   <si>
     <t>Task</t>
   </si>
@@ -96,18 +97,6 @@
   </si>
   <si>
     <t>Version</t>
-  </si>
-  <si>
-    <t>CPU ARM</t>
-  </si>
-  <si>
-    <t>CPU AMD</t>
-  </si>
-  <si>
-    <t>FPGA (optimized)</t>
-  </si>
-  <si>
-    <t>FPGA (baseline)</t>
   </si>
   <si>
     <t>1280x720
@@ -134,27 +123,6 @@
 CGA</t>
   </si>
   <si>
-    <t>Everything on CPU</t>
-  </si>
-  <si>
-    <t>Everything on FPGA</t>
-  </si>
-  <si>
-    <t>Baseline</t>
-  </si>
-  <si>
-    <t>Optimized</t>
-  </si>
-  <si>
-    <t>Trivial Partitioning Scheme</t>
-  </si>
-  <si>
-    <t>Speedup of Optimized vs. Baseline</t>
-  </si>
-  <si>
-    <t>Exec Time Estimate (us)</t>
-  </si>
-  <si>
     <t>HW/SW Partitioning Results</t>
   </si>
   <si>
@@ -186,14 +154,85 @@
   </si>
   <si>
     <t>Speedup vs. FPGA-only:</t>
+  </si>
+  <si>
+    <t>edge_detect_localdata</t>
+  </si>
+  <si>
+    <t>convolve2d_fused</t>
+  </si>
+  <si>
+    <t>7.3x</t>
+  </si>
+  <si>
+    <t>ED-B</t>
+  </si>
+  <si>
+    <t>ED-O1</t>
+  </si>
+  <si>
+    <t>ED-O2</t>
+  </si>
+  <si>
+    <t>Speedup vs. ED-B</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>ExecTime (us)</t>
+  </si>
+  <si>
+    <t>Trivial Partitioning</t>
+  </si>
+  <si>
+    <t>Everything on the CPU (P-SW)</t>
+  </si>
+  <si>
+    <t>Everything on the FPGA (P-HW)</t>
+  </si>
+  <si>
+    <t>P-SW</t>
+  </si>
+  <si>
+    <t>P-HW</t>
+  </si>
+  <si>
+    <t>FPGA (ED-B-D)</t>
+  </si>
+  <si>
+    <t>FPGA (ED-O1-D)</t>
+  </si>
+  <si>
+    <t>CPU AMD  (ED-B-D)</t>
+  </si>
+  <si>
+    <t>CPU ARM (ED-B-D)</t>
+  </si>
+  <si>
+    <t>vs. ED-O1 P-SW</t>
+  </si>
+  <si>
+    <t>vs. ED-O1 P-HW</t>
+  </si>
+  <si>
+    <t>vs. ED-B P-SW</t>
+  </si>
+  <si>
+    <t>vs. ED-B P-HW</t>
+  </si>
+  <si>
+    <t>vs. ED-B P-ILP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0\x"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.0\x"/>
+    <numFmt numFmtId="165" formatCode="0.00\x"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -344,7 +383,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -388,16 +427,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +491,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CPU AMD</c:v>
+                  <c:v>CPU AMD  (ED-B-D)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -591,7 +636,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CPU ARM</c:v>
+                  <c:v>CPU ARM (ED-B-D)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -736,7 +781,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FPGA (baseline)</c:v>
+                  <c:v>FPGA (ED-B-D)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -881,7 +926,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>FPGA (optimized)</c:v>
+                  <c:v>FPGA (ED-O1-D)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1191,7 +1236,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Execution time (us)</a:t>
+                  <a:t>Execution time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2408,17 +2453,17 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="27"/>
+      <c r="A12" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="28"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2426,7 +2471,7 @@
         <v>5</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2434,7 +2479,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2442,7 +2487,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2450,7 +2495,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2458,7 +2503,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2466,7 +2511,7 @@
         <v>3</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2474,7 +2519,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2482,28 +2527,28 @@
         <v>1</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B24">
         <v>71601</v>
@@ -2511,7 +2556,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B25">
         <v>15090</v>
@@ -2519,7 +2564,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B26" s="7">
         <v>0.21075124649097079</v>
@@ -2527,17 +2572,17 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" s="30">
+        <v>34</v>
+      </c>
+      <c r="B27" s="27">
         <v>6.0805296015418779</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" s="30">
+        <v>35</v>
+      </c>
+      <c r="B28" s="27">
         <v>97.049701126573893</v>
       </c>
     </row>
@@ -2552,10 +2597,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B033A240-9DD8-410C-BFF1-B3FA28355E0B}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="A23:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2703,7 +2748,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2711,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2719,7 +2764,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2727,7 +2772,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2735,7 +2780,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2743,7 +2788,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2751,63 +2796,99 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>32294</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B19">
         <v>7570</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B20" s="7">
         <v>0.23440886852046819</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" s="30">
+        <v>54</v>
+      </c>
+      <c r="B21" s="27">
         <v>14.72731776800644</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="30">
+        <v>55</v>
+      </c>
+      <c r="B22" s="27">
         <v>6.1987873183619548</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="34">
+        <f>C23/$B$18</f>
+        <v>13.481513593856445</v>
+      </c>
+      <c r="C23">
+        <v>435372</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="34">
+        <f t="shared" ref="B24:B25" si="0">C24/$B$18</f>
+        <v>45.348330959311326</v>
+      </c>
+      <c r="C24">
+        <v>1464479</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B25" s="34">
+        <f t="shared" si="0"/>
+        <v>2.2171610825540347</v>
+      </c>
+      <c r="C25">
+        <v>71601</v>
       </c>
     </row>
   </sheetData>
@@ -2816,11 +2897,284 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{626F9B67-CF83-4FF7-B6D1-65711B8B9603}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>149827</v>
+      </c>
+      <c r="C2" s="8">
+        <v>7866.1900000000005</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1.3271672504378201E-2</v>
+      </c>
+      <c r="E2" s="7">
+        <v>5.0492556917688197E-2</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>5.5555555555555497E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>17706</v>
+      </c>
+      <c r="C3" s="8">
+        <v>23410.43</v>
+      </c>
+      <c r="D3" s="7">
+        <v>3.3986427320490298E-3</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1.04057209573847E-2</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>22430</v>
+      </c>
+      <c r="C4" s="8">
+        <v>20809.46</v>
+      </c>
+      <c r="D4" s="7">
+        <v>4.13852012314823E-3</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1.01469087227782E-2</v>
+      </c>
+      <c r="F4" s="7">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>270074</v>
+      </c>
+      <c r="C5" s="3">
+        <v>5244.35</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7.8309252772912993E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.1555750145942701E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>58873</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>10578</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>0.1796748934146383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="27">
+        <v>3.4524409151068252</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="34">
+        <f>C21/$B$16</f>
+        <v>7.3951047169330595</v>
+      </c>
+      <c r="C21">
+        <v>435372</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="34">
+        <f t="shared" ref="B22:B23" si="0">C22/$B$16</f>
+        <v>24.875222937509555</v>
+      </c>
+      <c r="C22">
+        <v>1464479</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="34">
+        <f t="shared" si="0"/>
+        <v>1.2161941806940364</v>
+      </c>
+      <c r="C23">
+        <v>71601</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331B22D8-CD89-4FE0-A2AE-D35B65AF38CC}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2837,27 +3191,27 @@
     <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="22"/>
       <c r="B1" s="24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E1" s="24" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F1" s="24" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B2" s="25">
         <v>10.192200000000001</v>
@@ -2880,7 +3234,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B3" s="25">
         <v>28.3752</v>
@@ -2903,7 +3257,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="B4" s="25">
         <v>92.747600000000006</v>
@@ -2926,7 +3280,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B5" s="25">
         <v>85.691999999999993</v>
@@ -2954,93 +3308,221 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5AC4079-37DD-4400-BCFE-0CE8D2B084B0}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="A1:D5"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>29</v>
+      <c r="A2" s="31" t="s">
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C2">
         <v>435372</v>
       </c>
-      <c r="D2" s="29">
-        <f>C2/C3</f>
-        <v>0.91540861725300882</v>
+      <c r="D2" s="32" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+      <c r="A3" s="31"/>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <v>475604</v>
       </c>
-      <c r="D3" s="29"/>
+      <c r="D3" s="33">
+        <f>$C$2/C3</f>
+        <v>0.91540861725300882</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
-        <v>30</v>
-      </c>
+      <c r="A4" s="31"/>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C4">
+        <v>430172</v>
+      </c>
+      <c r="D4" s="33">
+        <f>$C$2/C4</f>
+        <v>1.0120881879806216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
         <v>1464479</v>
       </c>
-      <c r="D4" s="29">
-        <f>C4/C5</f>
+      <c r="D5" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="31"/>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6">
+        <v>46924</v>
+      </c>
+      <c r="D6" s="33">
+        <f>$C$5/C6</f>
         <v>31.209594237490411</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="31"/>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7">
+        <v>36520</v>
+      </c>
+      <c r="D7" s="33">
+        <f>$C$5/C7</f>
+        <v>40.100739320920042</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11">
+        <v>435372</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="29"/>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12">
+        <v>1464479</v>
+      </c>
+      <c r="D12" s="32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13">
+        <v>475604</v>
+      </c>
+      <c r="D13" s="33">
+        <f>$C$11/C13</f>
+        <v>0.91540861725300882</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="29"/>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14">
         <v>46924</v>
       </c>
-      <c r="D5" s="29"/>
+      <c r="D14" s="33">
+        <f>$C$12/C14</f>
+        <v>31.209594237490411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15">
+        <v>430172</v>
+      </c>
+      <c r="D15" s="33">
+        <f>$C$11/C15</f>
+        <v>1.0120881879806216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16">
+        <v>36520</v>
+      </c>
+      <c r="D16" s="33">
+        <f>$C$12/C16</f>
+        <v>40.100739320920042</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D4:D5"/>
+  <mergeCells count="5">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>